<commit_message>
Added sample computation for category averages
</commit_message>
<xml_diff>
--- a/Pageant Score Example.xlsx
+++ b/Pageant Score Example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarkIan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Visual Basic.Net\AMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>JD</t>
   </si>
@@ -401,15 +401,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -431,8 +431,23 @@
       <c r="I1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -455,8 +470,28 @@
         <f>AVERAGE(B2,C2,D2,E2,F2)</f>
         <v>82.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f>AVERAGE(B2,B14,B26)</f>
+        <v>81</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(C2,C14,C26)</f>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(D2,D14,D26)</f>
+        <v>84.333333333333329</v>
+      </c>
+      <c r="M2">
+        <f>AVERAGE(E2,E14,E26)</f>
+        <v>88.333333333333329</v>
+      </c>
+      <c r="N2">
+        <f>AVERAGE(F2,F14,F26)</f>
+        <v>85.666666666666671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -479,8 +514,28 @@
         <f t="shared" ref="H3:H12" si="0">AVERAGE(B3,C3,D3,E3,F3)</f>
         <v>87.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f>AVERAGE(B3,B15,B27)</f>
+        <v>88</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K12" si="1">AVERAGE(C3,C15,C27)</f>
+        <v>89.333333333333329</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L12" si="2">AVERAGE(D3,D15,D27)</f>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M12" si="3">AVERAGE(E3,E15,E27)</f>
+        <v>89.666666666666671</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N12" si="4">AVERAGE(F3,F15,F27)</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -503,8 +558,28 @@
         <f t="shared" si="0"/>
         <v>80.599999999999994</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f t="shared" ref="J3:J17" si="5">AVERAGE(B4,B16,B28)</f>
+        <v>86.333333333333329</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>81.666666666666671</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>83.666666666666671</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="3"/>
+        <v>85.333333333333329</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="4"/>
+        <v>85.666666666666671</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -527,8 +602,28 @@
         <f t="shared" si="0"/>
         <v>78.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f t="shared" si="5"/>
+        <v>85</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>87.666666666666671</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="4"/>
+        <v>86.666666666666671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -551,8 +646,28 @@
         <f t="shared" si="0"/>
         <v>94.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>94</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>94.666666666666671</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>92.666666666666671</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>94.333333333333329</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>92.666666666666671</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -575,8 +690,28 @@
         <f t="shared" si="0"/>
         <v>91.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>89</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>90.333333333333329</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>92.333333333333329</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>88.666666666666671</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -599,8 +734,28 @@
         <f t="shared" si="0"/>
         <v>87.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f t="shared" si="5"/>
+        <v>90.333333333333329</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>89.666666666666671</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>88.333333333333329</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -623,8 +778,28 @@
         <f t="shared" si="0"/>
         <v>91.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f t="shared" si="5"/>
+        <v>89.666666666666671</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>90.333333333333329</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>91.666666666666671</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>89.333333333333329</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>88.333333333333329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -647,8 +822,28 @@
         <f t="shared" si="0"/>
         <v>84.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f t="shared" si="5"/>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>85.333333333333329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -671,8 +866,28 @@
         <f t="shared" si="0"/>
         <v>92.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>92.333333333333329</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>92.666666666666671</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>92.666666666666671</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>90.333333333333329</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>93.666666666666671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -696,7 +911,7 @@
         <v>86.6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -716,11 +931,11 @@
         <v>91</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:H36" si="1">AVERAGE(B15,C15,D15,E15,F15)</f>
+        <f t="shared" ref="H15:H36" si="6">AVERAGE(B15,C15,D15,E15,F15)</f>
         <v>88.8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -740,7 +955,7 @@
         <v>82</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>84.8</v>
       </c>
     </row>
@@ -764,7 +979,7 @@
         <v>86</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
     </row>
@@ -788,7 +1003,7 @@
         <v>93</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>94.4</v>
       </c>
     </row>
@@ -812,7 +1027,7 @@
         <v>87</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
     </row>
@@ -836,7 +1051,7 @@
         <v>91</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>92.2</v>
       </c>
     </row>
@@ -860,7 +1075,7 @@
         <v>90</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
     </row>
@@ -884,7 +1099,7 @@
         <v>85</v>
       </c>
       <c r="H23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>86.2</v>
       </c>
     </row>
@@ -908,7 +1123,7 @@
         <v>94</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>93.2</v>
       </c>
     </row>
@@ -932,7 +1147,7 @@
         <v>89</v>
       </c>
       <c r="H26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>86.8</v>
       </c>
       <c r="I26" s="1">
@@ -960,11 +1175,11 @@
         <v>90</v>
       </c>
       <c r="H27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>88.6</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" ref="I27:I37" si="2">AVERAGE(H3,H15,H27)</f>
+        <f t="shared" ref="I27:I36" si="7">AVERAGE(H3,H15,H27)</f>
         <v>88.333333333333329</v>
       </c>
     </row>
@@ -988,11 +1203,11 @@
         <v>90</v>
       </c>
       <c r="H28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>88.2</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>84.533333333333317</v>
       </c>
     </row>
@@ -1016,11 +1231,11 @@
         <v>87</v>
       </c>
       <c r="H29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>87</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>85.333333333333329</v>
       </c>
     </row>
@@ -1044,11 +1259,11 @@
         <v>91</v>
       </c>
       <c r="H30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>92.4</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>93.666666666666671</v>
       </c>
     </row>
@@ -1075,11 +1290,11 @@
         <v>91</v>
       </c>
       <c r="H32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>89</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>90.066666666666663</v>
       </c>
     </row>
@@ -1103,11 +1318,11 @@
         <v>92</v>
       </c>
       <c r="H33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>89.866666666666674</v>
       </c>
     </row>
@@ -1131,11 +1346,11 @@
         <v>89</v>
       </c>
       <c r="H34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>88.2</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>89.866666666666674</v>
       </c>
     </row>
@@ -1159,11 +1374,11 @@
         <v>82</v>
       </c>
       <c r="H35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>84.8</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>85.2</v>
       </c>
     </row>
@@ -1187,11 +1402,11 @@
         <v>92</v>
       </c>
       <c r="H36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>91.4</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>92.333333333333329</v>
       </c>
     </row>

</xml_diff>